<commit_message>
fix xlsx2csv component, check relations between sheets
</commit_message>
<xml_diff>
--- a/flow/helloworld/test.xlsx
+++ b/flow/helloworld/test.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6280"/>
+    <workbookView windowWidth="19200" windowHeight="6280" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="aaa" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -985,7 +985,7 @@
   <sheetPr/>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -1052,14 +1052,13 @@
   <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix xlsx2csv component, manage empty cell values
</commit_message>
<xml_diff>
--- a/flow/helloworld/test.xlsx
+++ b/flow/helloworld/test.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>this</t>
   </si>
@@ -53,6 +53,18 @@
   </si>
   <si>
     <t>nontest</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
   </si>
 </sst>
 </file>
@@ -1050,14 +1062,44 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelRow="3" outlineLevelCol="4"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="5:5">
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>